<commit_message>
guia de implantação e diagrama de deployment
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/IFSP_Anote - Checklist Verificacao de Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/IFSP_Anote - Checklist Verificacao de Projeto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="117">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>Foram criados os testes unitários dos controladores?</t>
-  </si>
-  <si>
-    <t>Parcialmente</t>
   </si>
   <si>
     <t>Os testes unitários foram executados?</t>
@@ -1697,7 +1694,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.962962962962963</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.04761904761905</c:v>
@@ -2652,7 +2649,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -2765,7 +2762,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4836,7 +4833,7 @@
       </c>
       <c r="B4" s="60">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.962962962962963</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="14.4" spans="1:2">
@@ -6648,11 +6645,11 @@
       </c>
       <c r="O9" s="55">
         <f ca="1">('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="P9" s="55">
         <f ca="1">('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="55">
         <f ca="1">('Ver-Elaboração1'!$I$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
@@ -8297,7 +8294,7 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -16797,8 +16794,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -16837,7 +16834,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="8">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.962962962962963</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:6">
@@ -17255,11 +17252,11 @@
       <c r="F23" s="21"/>
       <c r="G23" s="23">
         <f>COUNTIF(D23:D27,"Sim")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H23" s="23">
         <f>COUNTIF(D23:D27,"Parcialmente")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="23">
         <f>COUNTIF(D23:D27,"Não")</f>
@@ -17307,7 +17304,7 @@
         <v>88</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
@@ -17318,7 +17315,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="34" t="s">
         <v>46</v>
@@ -17328,7 +17325,7 @@
     </row>
     <row r="28" ht="18.75" customHeight="1" spans="1:6">
       <c r="A28" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="17" t="s">
@@ -17344,7 +17341,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" s="34" t="s">
         <v>46</v>
@@ -17374,7 +17371,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30" s="34" t="s">
         <v>46</v>
@@ -17388,7 +17385,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31" s="34" t="s">
         <v>46</v>
@@ -17402,7 +17399,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>46</v>
@@ -17416,7 +17413,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="34" t="s">
         <v>46</v>
@@ -17430,7 +17427,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>46</v>
@@ -17524,7 +17521,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>46</v>
@@ -17554,7 +17551,7 @@
         <v>33</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>46</v>
@@ -19370,7 +19367,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>43</v>
@@ -19450,7 +19447,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>46</v>
@@ -19492,7 +19489,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>43</v>
@@ -19564,7 +19561,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>46</v>
@@ -19574,7 +19571,7 @@
     </row>
     <row r="23" ht="18.75" customHeight="1" spans="1:6">
       <c r="A23" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="17" t="s">
@@ -19620,7 +19617,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>46</v>
@@ -19634,7 +19631,7 @@
         <v>19</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>46</v>
@@ -19648,7 +19645,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>46</v>
@@ -19662,7 +19659,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>46</v>
@@ -19672,7 +19669,7 @@
     </row>
     <row r="29" ht="18.75" customHeight="1" spans="1:6">
       <c r="A29" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="17" t="s">
@@ -19688,7 +19685,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>46</v>
@@ -19718,7 +19715,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>46</v>
@@ -19732,7 +19729,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>46</v>
@@ -19746,7 +19743,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>46</v>
@@ -19760,7 +19757,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>46</v>
@@ -19842,7 +19839,7 @@
       <c r="A39" s="30"/>
       <c r="B39" s="20"/>
       <c r="C39" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>46</v>
@@ -19866,7 +19863,7 @@
         <v>33</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>46</v>
@@ -19896,7 +19893,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>46</v>
@@ -21685,7 +21682,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="21"/>
@@ -21759,7 +21756,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="21"/>
@@ -21799,7 +21796,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
@@ -21827,7 +21824,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="21"/>
@@ -21851,7 +21848,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="21"/>
@@ -21859,7 +21856,7 @@
     </row>
     <row r="22" ht="18.75" customHeight="1" spans="1:6">
       <c r="A22" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="17" t="s">
@@ -21875,7 +21872,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="21"/>
@@ -21903,7 +21900,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="21"/>
@@ -21911,7 +21908,7 @@
     </row>
     <row r="25" customHeight="1" spans="1:26">
       <c r="A25" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="17" t="s">
@@ -21991,7 +21988,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="21"/>
@@ -22057,7 +22054,7 @@
     </row>
     <row r="30" ht="18.75" customHeight="1" spans="1:6">
       <c r="A30" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="17" t="s">
@@ -22073,7 +22070,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="21"/>
@@ -22101,7 +22098,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="21"/>
@@ -22113,7 +22110,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="21"/>
@@ -22125,7 +22122,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="21"/>
@@ -22137,7 +22134,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="21"/>
@@ -22211,7 +22208,7 @@
       <c r="A40" s="30"/>
       <c r="B40" s="20"/>
       <c r="C40" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="21"/>
@@ -22233,7 +22230,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="21"/>
@@ -22261,7 +22258,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="21"/>

</xml_diff>